<commit_message>
Corrige base de datos de morfometría
</commit_message>
<xml_diff>
--- a/tests/data/datos_pruebas_sin_errores/IG_MORFOMETRIA_GATOS_14JUN2020.xlsx
+++ b/tests/data/datos_pruebas_sin_errores/IG_MORFOMETRIA_GATOS_14JUN2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
   <si>
     <t xml:space="preserve">Fecha</t>
   </si>
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">09-Junio-2020</t>
+    <t xml:space="preserve">09/Jun/2020</t>
   </si>
   <si>
     <t xml:space="preserve">TC-01-048-AG</t>
@@ -169,7 +169,7 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">Erradicaion</t>
+    <t xml:space="preserve">Erradicacion</t>
   </si>
   <si>
     <t xml:space="preserve">Sano</t>
@@ -181,13 +181,13 @@
     <t xml:space="preserve">A la cria no se le aplico la eutanasia porque sera donada. </t>
   </si>
   <si>
-    <t xml:space="preserve">10-junio-2020</t>
+    <t xml:space="preserve">10/Jun/2020</t>
   </si>
   <si>
     <t xml:space="preserve">TC-01-166-AG</t>
   </si>
   <si>
-    <t xml:space="preserve">378989 </t>
+    <t xml:space="preserve">378989</t>
   </si>
   <si>
     <t xml:space="preserve">3198524</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">1.6</t>
   </si>
   <si>
-    <t xml:space="preserve">11-Junio-2020</t>
+    <t xml:space="preserve">11/Jun/2020</t>
   </si>
   <si>
     <t xml:space="preserve">TC-03-135-NN</t>
@@ -339,12 +339,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -438,11 +438,11 @@
   </sheetPr>
   <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AD2" activeCellId="0" sqref="AD2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="94" zoomScaleNormal="94" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K4" activeCellId="0" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.85"/>
@@ -450,11 +450,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="18.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="19.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="10" style="1" width="8.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="23.15"/>
@@ -574,10 +574,10 @@
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -675,10 +675,10 @@
       <c r="C3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>56</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -695,6 +695,9 @@
       </c>
       <c r="J3" s="1" t="s">
         <v>60</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>61</v>
@@ -764,7 +767,7 @@
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -800,25 +803,25 @@
       <c r="M4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="5" t="s">
+      <c r="N4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="P4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="T4" s="5" t="s">
+      <c r="P4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>72</v>
       </c>
       <c r="U4" s="1" t="s">
@@ -833,7 +836,7 @@
       <c r="X4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="Y4" s="5" t="s">
+      <c r="Y4" s="6" t="s">
         <v>51</v>
       </c>
       <c r="Z4" s="1" t="s">

</xml_diff>